<commit_message>
More Testing with Git
</commit_message>
<xml_diff>
--- a/Blue Bell Ice Cream Needs.xlsx
+++ b/Blue Bell Ice Cream Needs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clearstar-my.sharepoint.com/personal/brians_clearstar_net/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brians\gittutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5341901-E1A6-45C3-BE59-C3ABA25A1502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7E727-50EB-4FAF-A6FF-27D7BCFCA879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60315" yWindow="1320" windowWidth="21600" windowHeight="11325" xr2:uid="{1850FA9C-0699-4CB6-9662-127EAE606AB9}"/>
+    <workbookView xWindow="58368" yWindow="768" windowWidth="21600" windowHeight="11448" xr2:uid="{1850FA9C-0699-4CB6-9662-127EAE606AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>PASSWORD 16 upsb?nQF&gt;D27GTSg</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>J*N4EmR8p6v?eSM&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,6 +647,16 @@
         <v>38</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>0</v>

</xml_diff>